<commit_message>
backend/sdoc: finish migration, removing all instances of REFS
</commit_message>
<xml_diff>
--- a/tests/integration/backend/excel/export/06_custom_grammar_fields_to_export_fields_all/expected/input.xlsx
+++ b/tests/integration/backend/excel/export/06_custom_grammar_fields_to_export_fields_all/expected/input.xlsx
@@ -34,8 +34,7 @@
     <t>REQ-002</t>
   </si>
   <si>
-    <t xml:space="preserve">Parent: REQ-001
-</t>
+    <t>Parent: REQ-001</t>
   </si>
   <si>
     <t>Title #2</t>
@@ -53,8 +52,9 @@
     <t>REQ-003</t>
   </si>
   <si>
-    <t xml:space="preserve">Parent: REQ-002
-</t>
+    <t>Parent: REQ-001
+----
+Parent: REQ-002</t>
   </si>
   <si>
     <t>Title #3</t>
@@ -69,7 +69,7 @@
     <t>UID</t>
   </si>
   <si>
-    <t>REFS</t>
+    <t>RELATIONS</t>
   </si>
   <si>
     <t>TITLE</t>
@@ -133,7 +133,7 @@
   <autoFilter ref="A1:F4"/>
   <tableColumns count="6">
     <tableColumn id="1" name="UID"/>
-    <tableColumn id="2" name="REFS"/>
+    <tableColumn id="2" name="RELATIONS"/>
     <tableColumn id="3" name="TITLE"/>
     <tableColumn id="4" name="STATEMENT"/>
     <tableColumn id="5" name="OWNER"/>
@@ -435,7 +435,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" customWidth="1"/>

</xml_diff>